<commit_message>
Update Numbers and Names of Databases in CrossAsia.xlsx
</commit_message>
<xml_diff>
--- a/CrossAsia/Numbers and Names of Databases in CrossAsia.xlsx
+++ b/CrossAsia/Numbers and Names of Databases in CrossAsia.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="196">
   <si>
     <t>CrossAsia</t>
   </si>
@@ -599,6 +599,18 @@
   </si>
   <si>
     <t>民国报纸 数字化</t>
+  </si>
+  <si>
+    <t>OCR</t>
+  </si>
+  <si>
+    <t>OCR 民国</t>
+  </si>
+  <si>
+    <t>OCR 古籍</t>
+  </si>
+  <si>
+    <t>光学字符识别</t>
   </si>
 </sst>
 </file>
@@ -633,7 +645,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -773,11 +785,117 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -848,19 +966,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2106,9 +2238,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2182,7 +2316,7 @@
         <v>176</v>
       </c>
       <c r="B4" s="30">
-        <f t="shared" ref="B4:B17" si="0">C4+F4</f>
+        <f t="shared" ref="B4:B22" si="0">C4+F4</f>
         <v>110</v>
       </c>
       <c r="C4" s="31">
@@ -2643,16 +2777,103 @@
       <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="28"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="34"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="42">
+        <f t="shared" si="0"/>
+        <v>1271</v>
+      </c>
+      <c r="C19" s="41">
+        <v>1151</v>
+      </c>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="44">
+        <v>120</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="43"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="30">
+        <f t="shared" si="0"/>
+        <v>6209</v>
+      </c>
+      <c r="C20" s="38">
+        <v>5254</v>
+      </c>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="48">
+        <v>955</v>
+      </c>
+      <c r="G20" s="46"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="47"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="30">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C21" s="38">
+        <v>4</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="48">
+        <v>1</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="47"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="50">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C22" s="51">
+        <v>15</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="54">
+        <v>17</v>
+      </c>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>